<commit_message>
making sure the patient records for adult and paed are also imported
</commit_message>
<xml_diff>
--- a/dashboard/tests/fixtures/new_format.xlsx
+++ b/dashboard/tests/fixtures/new_format.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Reporting facilities" sheetId="1" r:id="rId1"/>
     <sheet name="CONSUMPTION" sheetId="2" r:id="rId2"/>
+    <sheet name="PATIENTS (ADULT)" sheetId="3" r:id="rId3"/>
+    <sheet name="PATIENTS (PAED)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" calcMode="manual" calcCompleted="0" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="139">
   <si>
     <t>Facility</t>
   </si>
@@ -319,6 +321,129 @@
   </si>
   <si>
     <t>Gulu Regional Referal Hospital_Gulu _Zidovudine/Lamivudine/Nevirapine (AZT/3TC/NVP) 300mg/150mg/200mg [Pack 60]</t>
+  </si>
+  <si>
+    <t>Existing</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>ABC/3TC/EFV</t>
+  </si>
+  <si>
+    <t>ABC/3TC/LPV/r</t>
+  </si>
+  <si>
+    <t>ABC/3TC/NVP</t>
+  </si>
+  <si>
+    <t>AZT/3TC/ABC</t>
+  </si>
+  <si>
+    <t>AZT/3TC/EFV</t>
+  </si>
+  <si>
+    <t>AZT/3TC/LPV/r</t>
+  </si>
+  <si>
+    <t>AZT/3TC/NVP</t>
+  </si>
+  <si>
+    <t>Abako HC III</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alebtong </t>
+  </si>
+  <si>
+    <t>Abako Subcounty</t>
+  </si>
+  <si>
+    <t>Abarilela HC III</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amuria </t>
+  </si>
+  <si>
+    <t>Abarilela Subcounty</t>
+  </si>
+  <si>
+    <t>Abim HOSPITAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abim </t>
+  </si>
+  <si>
+    <t>Abim Town Council</t>
+  </si>
+  <si>
+    <t>TDF/3TC/ATV/r (ADULT)</t>
+  </si>
+  <si>
+    <t>TDF/3TC/EFV (ADULT)</t>
+  </si>
+  <si>
+    <t>TDF/3TC/LPV/r (ADULT)</t>
+  </si>
+  <si>
+    <t>TDF/3TC/NVP (ADULT)</t>
+  </si>
+  <si>
+    <t>AZT/3TC/ATV/r (ADULT)</t>
+  </si>
+  <si>
+    <t>AZT/3TC/EFV (ADULT)</t>
+  </si>
+  <si>
+    <t>AZT/3TC/LPV/r (ADULT)</t>
+  </si>
+  <si>
+    <t>ABC/3TC/EFV (ADULT)</t>
+  </si>
+  <si>
+    <t>ABC/3TC/NVP (ADULT)</t>
+  </si>
+  <si>
+    <t>AZT/3TC/NVP (ADULT)</t>
+  </si>
+  <si>
+    <t>ABC/3TC/AZT (ADULT)</t>
+  </si>
+  <si>
+    <t>TDF/3TC/AZT (ADULT)</t>
+  </si>
+  <si>
+    <t>ABC/3TC/ATV/r (ADULT)</t>
+  </si>
+  <si>
+    <t>ABC/3TC/LPV/r (ADULT)</t>
+  </si>
+  <si>
+    <t>ABC/3TC/AZT (PMTCT)</t>
+  </si>
+  <si>
+    <t>ABC/3TC/EFV (PMTCT)</t>
+  </si>
+  <si>
+    <t>ABC/3TC/NVP (PMTCT)</t>
+  </si>
+  <si>
+    <t>AZT/3TC/EFV (PMTCT)</t>
+  </si>
+  <si>
+    <t>AZT/3TC/NVP (PMTCT)</t>
+  </si>
+  <si>
+    <t>TDF/3TC/AZT (PMTCT)</t>
+  </si>
+  <si>
+    <t>TDF/3TC/EFV (PMTCT)</t>
+  </si>
+  <si>
+    <t>TDF/3TC/NVP (PMTCT)</t>
   </si>
 </sst>
 </file>
@@ -707,7 +832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
@@ -3597,4 +3722,3205 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:M46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <v>170</v>
+      </c>
+      <c r="F4">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <v>52</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>80</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" t="s">
+        <v>26</v>
+      </c>
+      <c r="L14" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" t="s">
+        <v>26</v>
+      </c>
+      <c r="L15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" t="s">
+        <v>27</v>
+      </c>
+      <c r="M16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" t="s">
+        <v>26</v>
+      </c>
+      <c r="L17" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" t="s">
+        <v>26</v>
+      </c>
+      <c r="L18" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19" t="s">
+        <v>27</v>
+      </c>
+      <c r="M19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" t="s">
+        <v>26</v>
+      </c>
+      <c r="L20" t="s">
+        <v>27</v>
+      </c>
+      <c r="M20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" t="s">
+        <v>26</v>
+      </c>
+      <c r="L21" t="s">
+        <v>27</v>
+      </c>
+      <c r="M21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>136</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" t="s">
+        <v>25</v>
+      </c>
+      <c r="K22" t="s">
+        <v>26</v>
+      </c>
+      <c r="L22" t="s">
+        <v>27</v>
+      </c>
+      <c r="M22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23">
+        <v>9</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+      <c r="G23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" t="s">
+        <v>25</v>
+      </c>
+      <c r="K23" t="s">
+        <v>26</v>
+      </c>
+      <c r="L23" t="s">
+        <v>27</v>
+      </c>
+      <c r="M23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s">
+        <v>138</v>
+      </c>
+      <c r="D24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24" t="s">
+        <v>26</v>
+      </c>
+      <c r="L24" t="s">
+        <v>27</v>
+      </c>
+      <c r="M24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>117</v>
+      </c>
+      <c r="D25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25">
+        <v>94</v>
+      </c>
+      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="G25" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" t="s">
+        <v>55</v>
+      </c>
+      <c r="J25" t="s">
+        <v>56</v>
+      </c>
+      <c r="K25" t="s">
+        <v>26</v>
+      </c>
+      <c r="L25" t="s">
+        <v>27</v>
+      </c>
+      <c r="M25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26">
+        <v>4322</v>
+      </c>
+      <c r="F26">
+        <v>173</v>
+      </c>
+      <c r="G26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" t="s">
+        <v>54</v>
+      </c>
+      <c r="I26" t="s">
+        <v>55</v>
+      </c>
+      <c r="J26" t="s">
+        <v>56</v>
+      </c>
+      <c r="K26" t="s">
+        <v>26</v>
+      </c>
+      <c r="L26" t="s">
+        <v>27</v>
+      </c>
+      <c r="M26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27">
+        <v>319</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" t="s">
+        <v>55</v>
+      </c>
+      <c r="J27" t="s">
+        <v>56</v>
+      </c>
+      <c r="K27" t="s">
+        <v>26</v>
+      </c>
+      <c r="L27" t="s">
+        <v>27</v>
+      </c>
+      <c r="M27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28">
+        <v>490</v>
+      </c>
+      <c r="F28">
+        <v>15</v>
+      </c>
+      <c r="G28" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" t="s">
+        <v>54</v>
+      </c>
+      <c r="I28" t="s">
+        <v>55</v>
+      </c>
+      <c r="J28" t="s">
+        <v>56</v>
+      </c>
+      <c r="K28" t="s">
+        <v>26</v>
+      </c>
+      <c r="L28" t="s">
+        <v>27</v>
+      </c>
+      <c r="M28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" t="s">
+        <v>121</v>
+      </c>
+      <c r="D29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29">
+        <v>23</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" t="s">
+        <v>55</v>
+      </c>
+      <c r="J29" t="s">
+        <v>56</v>
+      </c>
+      <c r="K29" t="s">
+        <v>26</v>
+      </c>
+      <c r="L29" t="s">
+        <v>27</v>
+      </c>
+      <c r="M29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>122</v>
+      </c>
+      <c r="D30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30">
+        <v>1526</v>
+      </c>
+      <c r="F30">
+        <v>11</v>
+      </c>
+      <c r="G30" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" t="s">
+        <v>54</v>
+      </c>
+      <c r="I30" t="s">
+        <v>55</v>
+      </c>
+      <c r="J30" t="s">
+        <v>56</v>
+      </c>
+      <c r="K30" t="s">
+        <v>26</v>
+      </c>
+      <c r="L30" t="s">
+        <v>27</v>
+      </c>
+      <c r="M30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31">
+        <v>87</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" t="s">
+        <v>54</v>
+      </c>
+      <c r="I31" t="s">
+        <v>55</v>
+      </c>
+      <c r="J31" t="s">
+        <v>56</v>
+      </c>
+      <c r="K31" t="s">
+        <v>26</v>
+      </c>
+      <c r="L31" t="s">
+        <v>27</v>
+      </c>
+      <c r="M31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32">
+        <v>53</v>
+      </c>
+      <c r="F32">
+        <v>9</v>
+      </c>
+      <c r="G32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" t="s">
+        <v>54</v>
+      </c>
+      <c r="I32" t="s">
+        <v>55</v>
+      </c>
+      <c r="J32" t="s">
+        <v>56</v>
+      </c>
+      <c r="K32" t="s">
+        <v>26</v>
+      </c>
+      <c r="L32" t="s">
+        <v>27</v>
+      </c>
+      <c r="M32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33">
+        <v>23</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" t="s">
+        <v>54</v>
+      </c>
+      <c r="I33" t="s">
+        <v>55</v>
+      </c>
+      <c r="J33" t="s">
+        <v>56</v>
+      </c>
+      <c r="K33" t="s">
+        <v>26</v>
+      </c>
+      <c r="L33" t="s">
+        <v>27</v>
+      </c>
+      <c r="M33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34">
+        <v>2081</v>
+      </c>
+      <c r="F34">
+        <v>8</v>
+      </c>
+      <c r="G34" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" t="s">
+        <v>54</v>
+      </c>
+      <c r="I34" t="s">
+        <v>55</v>
+      </c>
+      <c r="J34" t="s">
+        <v>56</v>
+      </c>
+      <c r="K34" t="s">
+        <v>26</v>
+      </c>
+      <c r="L34" t="s">
+        <v>27</v>
+      </c>
+      <c r="M34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" t="s">
+        <v>127</v>
+      </c>
+      <c r="D35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" t="s">
+        <v>54</v>
+      </c>
+      <c r="I35" t="s">
+        <v>55</v>
+      </c>
+      <c r="J35" t="s">
+        <v>56</v>
+      </c>
+      <c r="K35" t="s">
+        <v>26</v>
+      </c>
+      <c r="L35" t="s">
+        <v>27</v>
+      </c>
+      <c r="M35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" t="s">
+        <v>54</v>
+      </c>
+      <c r="I36" t="s">
+        <v>55</v>
+      </c>
+      <c r="J36" t="s">
+        <v>56</v>
+      </c>
+      <c r="K36" t="s">
+        <v>26</v>
+      </c>
+      <c r="L36" t="s">
+        <v>27</v>
+      </c>
+      <c r="M36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37">
+        <v>10</v>
+      </c>
+      <c r="F37">
+        <v>4</v>
+      </c>
+      <c r="G37" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" t="s">
+        <v>54</v>
+      </c>
+      <c r="I37" t="s">
+        <v>55</v>
+      </c>
+      <c r="J37" t="s">
+        <v>56</v>
+      </c>
+      <c r="K37" t="s">
+        <v>26</v>
+      </c>
+      <c r="L37" t="s">
+        <v>27</v>
+      </c>
+      <c r="M37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" t="s">
+        <v>130</v>
+      </c>
+      <c r="D38" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38">
+        <v>18</v>
+      </c>
+      <c r="F38">
+        <v>3</v>
+      </c>
+      <c r="G38" t="s">
+        <v>22</v>
+      </c>
+      <c r="H38" t="s">
+        <v>54</v>
+      </c>
+      <c r="I38" t="s">
+        <v>55</v>
+      </c>
+      <c r="J38" t="s">
+        <v>56</v>
+      </c>
+      <c r="K38" t="s">
+        <v>26</v>
+      </c>
+      <c r="L38" t="s">
+        <v>27</v>
+      </c>
+      <c r="M38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" t="s">
+        <v>131</v>
+      </c>
+      <c r="D39" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" t="s">
+        <v>54</v>
+      </c>
+      <c r="I39" t="s">
+        <v>55</v>
+      </c>
+      <c r="J39" t="s">
+        <v>56</v>
+      </c>
+      <c r="K39" t="s">
+        <v>26</v>
+      </c>
+      <c r="L39" t="s">
+        <v>27</v>
+      </c>
+      <c r="M39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40" t="s">
+        <v>22</v>
+      </c>
+      <c r="H40" t="s">
+        <v>54</v>
+      </c>
+      <c r="I40" t="s">
+        <v>55</v>
+      </c>
+      <c r="J40" t="s">
+        <v>56</v>
+      </c>
+      <c r="K40" t="s">
+        <v>26</v>
+      </c>
+      <c r="L40" t="s">
+        <v>27</v>
+      </c>
+      <c r="M40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" t="s">
+        <v>133</v>
+      </c>
+      <c r="D41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41" t="s">
+        <v>54</v>
+      </c>
+      <c r="I41" t="s">
+        <v>55</v>
+      </c>
+      <c r="J41" t="s">
+        <v>56</v>
+      </c>
+      <c r="K41" t="s">
+        <v>26</v>
+      </c>
+      <c r="L41" t="s">
+        <v>27</v>
+      </c>
+      <c r="M41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" t="s">
+        <v>134</v>
+      </c>
+      <c r="D42" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42">
+        <v>44</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42" t="s">
+        <v>22</v>
+      </c>
+      <c r="H42" t="s">
+        <v>54</v>
+      </c>
+      <c r="I42" t="s">
+        <v>55</v>
+      </c>
+      <c r="J42" t="s">
+        <v>56</v>
+      </c>
+      <c r="K42" t="s">
+        <v>26</v>
+      </c>
+      <c r="L42" t="s">
+        <v>27</v>
+      </c>
+      <c r="M42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" t="s">
+        <v>135</v>
+      </c>
+      <c r="D43" t="s">
+        <v>22</v>
+      </c>
+      <c r="E43">
+        <v>10</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43" t="s">
+        <v>22</v>
+      </c>
+      <c r="H43" t="s">
+        <v>54</v>
+      </c>
+      <c r="I43" t="s">
+        <v>55</v>
+      </c>
+      <c r="J43" t="s">
+        <v>56</v>
+      </c>
+      <c r="K43" t="s">
+        <v>26</v>
+      </c>
+      <c r="L43" t="s">
+        <v>27</v>
+      </c>
+      <c r="M43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" t="s">
+        <v>136</v>
+      </c>
+      <c r="D44" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44" t="s">
+        <v>22</v>
+      </c>
+      <c r="H44" t="s">
+        <v>54</v>
+      </c>
+      <c r="I44" t="s">
+        <v>55</v>
+      </c>
+      <c r="J44" t="s">
+        <v>56</v>
+      </c>
+      <c r="K44" t="s">
+        <v>26</v>
+      </c>
+      <c r="L44" t="s">
+        <v>27</v>
+      </c>
+      <c r="M44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" t="s">
+        <v>137</v>
+      </c>
+      <c r="D45" t="s">
+        <v>22</v>
+      </c>
+      <c r="E45">
+        <v>673</v>
+      </c>
+      <c r="F45">
+        <v>61</v>
+      </c>
+      <c r="G45" t="s">
+        <v>22</v>
+      </c>
+      <c r="H45" t="s">
+        <v>54</v>
+      </c>
+      <c r="I45" t="s">
+        <v>55</v>
+      </c>
+      <c r="J45" t="s">
+        <v>56</v>
+      </c>
+      <c r="K45" t="s">
+        <v>26</v>
+      </c>
+      <c r="L45" t="s">
+        <v>27</v>
+      </c>
+      <c r="M45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" t="s">
+        <v>138</v>
+      </c>
+      <c r="D46" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46">
+        <v>30</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H46" t="s">
+        <v>54</v>
+      </c>
+      <c r="I46" t="s">
+        <v>55</v>
+      </c>
+      <c r="J46" t="s">
+        <v>56</v>
+      </c>
+      <c r="K46" t="s">
+        <v>26</v>
+      </c>
+      <c r="L46" t="s">
+        <v>27</v>
+      </c>
+      <c r="M46" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:N37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11">
+        <v>18</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>48</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14">
+        <v>73</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" t="s">
+        <v>26</v>
+      </c>
+      <c r="L14" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15">
+        <v>169</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" t="s">
+        <v>56</v>
+      </c>
+      <c r="K15" t="s">
+        <v>26</v>
+      </c>
+      <c r="L15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16">
+        <v>368</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" t="s">
+        <v>27</v>
+      </c>
+      <c r="M16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" t="s">
+        <v>108</v>
+      </c>
+      <c r="J17" t="s">
+        <v>109</v>
+      </c>
+      <c r="K17" t="s">
+        <v>26</v>
+      </c>
+      <c r="L17" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" t="s">
+        <v>28</v>
+      </c>
+      <c r="N17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" t="s">
+        <v>108</v>
+      </c>
+      <c r="J18" t="s">
+        <v>109</v>
+      </c>
+      <c r="K18" t="s">
+        <v>26</v>
+      </c>
+      <c r="L18" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" t="s">
+        <v>28</v>
+      </c>
+      <c r="N18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" t="s">
+        <v>108</v>
+      </c>
+      <c r="J19" t="s">
+        <v>109</v>
+      </c>
+      <c r="K19" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19" t="s">
+        <v>27</v>
+      </c>
+      <c r="M19" t="s">
+        <v>28</v>
+      </c>
+      <c r="N19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" t="s">
+        <v>108</v>
+      </c>
+      <c r="J20" t="s">
+        <v>109</v>
+      </c>
+      <c r="K20" t="s">
+        <v>26</v>
+      </c>
+      <c r="L20" t="s">
+        <v>27</v>
+      </c>
+      <c r="M20" t="s">
+        <v>28</v>
+      </c>
+      <c r="N20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" t="s">
+        <v>108</v>
+      </c>
+      <c r="J21" t="s">
+        <v>109</v>
+      </c>
+      <c r="K21" t="s">
+        <v>26</v>
+      </c>
+      <c r="L21" t="s">
+        <v>27</v>
+      </c>
+      <c r="M21" t="s">
+        <v>28</v>
+      </c>
+      <c r="N21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" t="s">
+        <v>54</v>
+      </c>
+      <c r="I22" t="s">
+        <v>108</v>
+      </c>
+      <c r="J22" t="s">
+        <v>109</v>
+      </c>
+      <c r="K22" t="s">
+        <v>26</v>
+      </c>
+      <c r="L22" t="s">
+        <v>27</v>
+      </c>
+      <c r="M22" t="s">
+        <v>28</v>
+      </c>
+      <c r="N22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" t="s">
+        <v>108</v>
+      </c>
+      <c r="J23" t="s">
+        <v>109</v>
+      </c>
+      <c r="K23" t="s">
+        <v>26</v>
+      </c>
+      <c r="L23" t="s">
+        <v>27</v>
+      </c>
+      <c r="M23" t="s">
+        <v>28</v>
+      </c>
+      <c r="N23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24">
+        <v>16</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" t="s">
+        <v>111</v>
+      </c>
+      <c r="I24" t="s">
+        <v>112</v>
+      </c>
+      <c r="J24" t="s">
+        <v>113</v>
+      </c>
+      <c r="K24" t="s">
+        <v>26</v>
+      </c>
+      <c r="L24" t="s">
+        <v>27</v>
+      </c>
+      <c r="M24" t="s">
+        <v>28</v>
+      </c>
+      <c r="N24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" t="s">
+        <v>111</v>
+      </c>
+      <c r="I25" t="s">
+        <v>112</v>
+      </c>
+      <c r="J25" t="s">
+        <v>113</v>
+      </c>
+      <c r="K25" t="s">
+        <v>26</v>
+      </c>
+      <c r="L25" t="s">
+        <v>27</v>
+      </c>
+      <c r="M25" t="s">
+        <v>28</v>
+      </c>
+      <c r="N25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" t="s">
+        <v>111</v>
+      </c>
+      <c r="I26" t="s">
+        <v>112</v>
+      </c>
+      <c r="J26" t="s">
+        <v>113</v>
+      </c>
+      <c r="K26" t="s">
+        <v>26</v>
+      </c>
+      <c r="L26" t="s">
+        <v>27</v>
+      </c>
+      <c r="M26" t="s">
+        <v>28</v>
+      </c>
+      <c r="N26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" t="s">
+        <v>111</v>
+      </c>
+      <c r="I27" t="s">
+        <v>112</v>
+      </c>
+      <c r="J27" t="s">
+        <v>113</v>
+      </c>
+      <c r="K27" t="s">
+        <v>26</v>
+      </c>
+      <c r="L27" t="s">
+        <v>27</v>
+      </c>
+      <c r="M27" t="s">
+        <v>28</v>
+      </c>
+      <c r="N27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" t="s">
+        <v>111</v>
+      </c>
+      <c r="I28" t="s">
+        <v>112</v>
+      </c>
+      <c r="J28" t="s">
+        <v>113</v>
+      </c>
+      <c r="K28" t="s">
+        <v>26</v>
+      </c>
+      <c r="L28" t="s">
+        <v>27</v>
+      </c>
+      <c r="M28" t="s">
+        <v>28</v>
+      </c>
+      <c r="N28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" t="s">
+        <v>111</v>
+      </c>
+      <c r="I29" t="s">
+        <v>112</v>
+      </c>
+      <c r="J29" t="s">
+        <v>113</v>
+      </c>
+      <c r="K29" t="s">
+        <v>26</v>
+      </c>
+      <c r="L29" t="s">
+        <v>27</v>
+      </c>
+      <c r="M29" t="s">
+        <v>28</v>
+      </c>
+      <c r="N29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30">
+        <v>6</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" t="s">
+        <v>111</v>
+      </c>
+      <c r="I30" t="s">
+        <v>112</v>
+      </c>
+      <c r="J30" t="s">
+        <v>113</v>
+      </c>
+      <c r="K30" t="s">
+        <v>26</v>
+      </c>
+      <c r="L30" t="s">
+        <v>27</v>
+      </c>
+      <c r="M30" t="s">
+        <v>28</v>
+      </c>
+      <c r="N30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31">
+        <v>11</v>
+      </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
+      <c r="G31" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" t="s">
+        <v>54</v>
+      </c>
+      <c r="I31" t="s">
+        <v>115</v>
+      </c>
+      <c r="J31" t="s">
+        <v>116</v>
+      </c>
+      <c r="K31" t="s">
+        <v>26</v>
+      </c>
+      <c r="L31" t="s">
+        <v>27</v>
+      </c>
+      <c r="M31" t="s">
+        <v>28</v>
+      </c>
+      <c r="N31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" t="s">
+        <v>54</v>
+      </c>
+      <c r="I32" t="s">
+        <v>115</v>
+      </c>
+      <c r="J32" t="s">
+        <v>116</v>
+      </c>
+      <c r="K32" t="s">
+        <v>26</v>
+      </c>
+      <c r="L32" t="s">
+        <v>27</v>
+      </c>
+      <c r="M32" t="s">
+        <v>28</v>
+      </c>
+      <c r="N32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>3</v>
+      </c>
+      <c r="G33" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" t="s">
+        <v>54</v>
+      </c>
+      <c r="I33" t="s">
+        <v>115</v>
+      </c>
+      <c r="J33" t="s">
+        <v>116</v>
+      </c>
+      <c r="K33" t="s">
+        <v>26</v>
+      </c>
+      <c r="L33" t="s">
+        <v>27</v>
+      </c>
+      <c r="M33" t="s">
+        <v>28</v>
+      </c>
+      <c r="N33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" t="s">
+        <v>103</v>
+      </c>
+      <c r="D34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" t="s">
+        <v>54</v>
+      </c>
+      <c r="I34" t="s">
+        <v>115</v>
+      </c>
+      <c r="J34" t="s">
+        <v>116</v>
+      </c>
+      <c r="K34" t="s">
+        <v>26</v>
+      </c>
+      <c r="L34" t="s">
+        <v>27</v>
+      </c>
+      <c r="M34" t="s">
+        <v>28</v>
+      </c>
+      <c r="N34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" t="s">
+        <v>104</v>
+      </c>
+      <c r="D35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" t="s">
+        <v>54</v>
+      </c>
+      <c r="I35" t="s">
+        <v>115</v>
+      </c>
+      <c r="J35" t="s">
+        <v>116</v>
+      </c>
+      <c r="K35" t="s">
+        <v>26</v>
+      </c>
+      <c r="L35" t="s">
+        <v>27</v>
+      </c>
+      <c r="M35" t="s">
+        <v>28</v>
+      </c>
+      <c r="N35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" t="s">
+        <v>54</v>
+      </c>
+      <c r="I36" t="s">
+        <v>115</v>
+      </c>
+      <c r="J36" t="s">
+        <v>116</v>
+      </c>
+      <c r="K36" t="s">
+        <v>26</v>
+      </c>
+      <c r="L36" t="s">
+        <v>27</v>
+      </c>
+      <c r="M36" t="s">
+        <v>28</v>
+      </c>
+      <c r="N36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" t="s">
+        <v>106</v>
+      </c>
+      <c r="D37" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37">
+        <v>47</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" t="s">
+        <v>54</v>
+      </c>
+      <c r="I37" t="s">
+        <v>115</v>
+      </c>
+      <c r="J37" t="s">
+        <v>116</v>
+      </c>
+      <c r="K37" t="s">
+        <v>26</v>
+      </c>
+      <c r="L37" t="s">
+        <v>27</v>
+      </c>
+      <c r="M37" t="s">
+        <v>28</v>
+      </c>
+      <c r="N37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cleared the migrations and setup location import
</commit_message>
<xml_diff>
--- a/dashboard/tests/fixtures/new_format.xlsx
+++ b/dashboard/tests/fixtures/new_format.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesmuranga/code/space/chai/evEnv/dashboard/tests/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesmuranga/code/space/chai/OrderQualityTool/dashboard/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Reporting facilities" sheetId="1" r:id="rId1"/>
+    <sheet name="Facility Index" sheetId="1" r:id="rId1"/>
     <sheet name="CONSUMPTION" sheetId="2" r:id="rId2"/>
     <sheet name="PATIENTS (ADULT)" sheetId="3" r:id="rId3"/>
     <sheet name="PATIENTS (PAED)" sheetId="4" r:id="rId4"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1574" uniqueCount="193">
   <si>
     <t>Facility</t>
   </si>
@@ -444,13 +444,175 @@
   </si>
   <si>
     <t>TDF/3TC/NVP (PMTCT)</t>
+  </si>
+  <si>
+    <t>Reference list:</t>
+  </si>
+  <si>
+    <t>STATIC Master list</t>
+  </si>
+  <si>
+    <t>Facility in THIS CYCLE</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>Multiple orders submitted?</t>
+  </si>
+  <si>
+    <t>Nkokonjeru HC III_Kayunga</t>
+  </si>
+  <si>
+    <t>Reporting</t>
+  </si>
+  <si>
+    <t>Walter Reed</t>
+  </si>
+  <si>
+    <t>Kayunga</t>
+  </si>
+  <si>
+    <t>Abarilela HC III_Amuria</t>
+  </si>
+  <si>
+    <t>UNICEF</t>
+  </si>
+  <si>
+    <t>Amuria</t>
+  </si>
+  <si>
+    <t>Abim HOSPITAL_Abim</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Abim</t>
+  </si>
+  <si>
+    <t>Acowa HC III_Amuria</t>
+  </si>
+  <si>
+    <t>Agu HC III_Ngora</t>
+  </si>
+  <si>
+    <t>Baylor</t>
+  </si>
+  <si>
+    <t>Ngora</t>
+  </si>
+  <si>
+    <t>Ajeluk HC III_Ngora</t>
+  </si>
+  <si>
+    <t>Multiple orders</t>
+  </si>
+  <si>
+    <t>Aketa HC III_Katakwi</t>
+  </si>
+  <si>
+    <t>UPMB</t>
+  </si>
+  <si>
+    <t>Katakwi</t>
+  </si>
+  <si>
+    <t>Alerek HC III_Abim</t>
+  </si>
+  <si>
+    <t>Alwa HC III_Kaberamaido</t>
+  </si>
+  <si>
+    <t>UCMB</t>
+  </si>
+  <si>
+    <t>Kaberamaido</t>
+  </si>
+  <si>
+    <t>Amolatar HC IV_Amolatar</t>
+  </si>
+  <si>
+    <t>NUHITES</t>
+  </si>
+  <si>
+    <t>Amolatar</t>
+  </si>
+  <si>
+    <t>Amoru HC III_Kaberamaido</t>
+  </si>
+  <si>
+    <t>Amuria HC IV_Amuria</t>
+  </si>
+  <si>
+    <t>Anyara HC III_Kaberamaido</t>
+  </si>
+  <si>
+    <t>Apapai HC IV_Serere</t>
+  </si>
+  <si>
+    <t>Mildmay</t>
+  </si>
+  <si>
+    <t>Serere</t>
+  </si>
+  <si>
+    <t>Apeitolim HC II_Napak</t>
+  </si>
+  <si>
+    <t>Star EC</t>
+  </si>
+  <si>
+    <t>Napak</t>
+  </si>
+  <si>
+    <t>Asamuk HC III_Amuria</t>
+  </si>
+  <si>
+    <t>Asuret HC III_Soroti</t>
+  </si>
+  <si>
+    <t>AIC</t>
+  </si>
+  <si>
+    <t>Soroti</t>
+  </si>
+  <si>
+    <t>Atiak HC IV_Amuru</t>
+  </si>
+  <si>
+    <t>Amuru</t>
+  </si>
+  <si>
+    <t>Atiira HC III_Serere</t>
+  </si>
+  <si>
+    <t>ATIRIR HC IV_Soroti</t>
+  </si>
+  <si>
+    <t>Atutur HOSPITAL_Kumi</t>
+  </si>
+  <si>
+    <t>Kumi</t>
+  </si>
+  <si>
+    <t>Balawoli HC III_Kamuli</t>
+  </si>
+  <si>
+    <t>Kamuli</t>
+  </si>
+  <si>
+    <t>Bbaale HC IV_Kayunga</t>
+  </si>
+  <si>
+    <t>Bibia HC III_Amuru</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -479,6 +641,32 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.2"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.2"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13.2"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -526,7 +714,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -541,6 +729,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,12 +1010,753 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="8"/>
+      <c r="B2" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+    </row>
+    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="8"/>
+      <c r="B7" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="H10" s="8"/>
+      <c r="I10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="H11" s="8"/>
+      <c r="I11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="B13" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="H14" s="8"/>
+      <c r="I14" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="H15" s="8"/>
+      <c r="I15" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="I16" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="H17" s="8"/>
+      <c r="I17" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
+      <c r="B18" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="H18" s="8"/>
+      <c r="I18" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="B19" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="H19" s="8"/>
+      <c r="I19" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+      <c r="B20" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="H20" s="8"/>
+      <c r="I20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="8"/>
+      <c r="B21" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="H21" s="8"/>
+      <c r="I21" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="8"/>
+      <c r="B22" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
+      <c r="B23" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="8"/>
+      <c r="B24" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="H24" s="8"/>
+      <c r="I24" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="H25" s="8"/>
+      <c r="I25" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="8"/>
+      <c r="B26" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="H26" s="8"/>
+      <c r="I26" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="8"/>
+      <c r="B27" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="H27" s="8"/>
+      <c r="I27" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+      <c r="B28" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="H28" s="8"/>
+      <c r="I28" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -832,7 +1765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X43"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
@@ -3728,7 +4661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changed the file import task to accomodate changes in the locations
</commit_message>
<xml_diff>
--- a/dashboard/tests/fixtures/new_format.xlsx
+++ b/dashboard/tests/fixtures/new_format.xlsx
@@ -1013,7 +1013,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1535,7 +1535,7 @@
     <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="11" t="s">
-        <v>180</v>
+        <v>20</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>180</v>
@@ -1647,7 +1647,7 @@
     <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>
       <c r="B25" s="11" t="s">
-        <v>187</v>
+        <v>53</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>187</v>

</xml_diff>

<commit_message>
caching the scores for the tests for each facility
</commit_message>
<xml_diff>
--- a/dashboard/tests/fixtures/new_format.xlsx
+++ b/dashboard/tests/fixtures/new_format.xlsx
@@ -17,7 +17,7 @@
     <sheet name="PATIENTS (ADULT)" sheetId="3" r:id="rId3"/>
     <sheet name="PATIENTS (PAED)" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150000" calcMode="manual" calcCompleted="0" concurrentCalc="0"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1013,7 +1013,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1731,7 +1731,7 @@
     <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="11" t="s">
-        <v>192</v>
+        <v>20</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>192</v>
@@ -1766,7 +1766,7 @@
   <dimension ref="A2:X43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>